<commit_message>
Conform to Google Drive
</commit_message>
<xml_diff>
--- a/2024-12-20 -- Promoted Associates.xlsx
+++ b/2024-12-20 -- Promoted Associates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reedsmith-my.sharepoint.com/personal/richard_robbins_reedsmith_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB484FCC-DFC1-403C-A5BC-C3238A97EFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{DB484FCC-DFC1-403C-A5BC-C3238A97EFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{630E61D6-A2F2-4484-A413-2BA06B1B96D8}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="3225" windowWidth="23715" windowHeight="17235" xr2:uid="{8672D67A-8712-4C2A-8134-37686E798F29}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17010" windowHeight="9870" xr2:uid="{8672D67A-8712-4C2A-8134-37686E798F29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Lowell P. Bourgeois</t>
   </si>
   <si>
-    <t>lowellbourgeois@gmail.com</t>
-  </si>
-  <si>
     <t>Katherine E. Geddes</t>
   </si>
   <si>
@@ -270,13 +267,16 @@
   </si>
   <si>
     <t>Email Address</t>
+  </si>
+  <si>
+    <t>lbourgeois@reedsmith.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -293,6 +293,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -313,21 +320,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,7 +673,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -674,317 +684,320 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{E6984C0C-5D53-446A-95D6-31400FB59483}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>